<commit_message>
Últimas entradas de horas
</commit_message>
<xml_diff>
--- a/Documentation/Project_Tracking/Task_Hour_Recount.xlsx
+++ b/Documentation/Project_Tracking/Task_Hour_Recount.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C805FF-CBC2-47AE-BB1A-398B232DD497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28CD304F-07F6-491C-B438-C6A155D109E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -105,6 +105,15 @@
   </si>
   <si>
     <t>Avances en multiples pantallas</t>
+  </si>
+  <si>
+    <t>Ultimas modificaciones del proyecto</t>
+  </si>
+  <si>
+    <t>Avances en multiples apartados</t>
+  </si>
+  <si>
+    <t>Ultimas modificaciones</t>
   </si>
 </sst>
 </file>
@@ -117,7 +126,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,6 +285,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Franklin Gothic Book"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -666,7 +683,7 @@
     <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -751,6 +768,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1053,8 +1073,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FDFFDC23-1EA5-434F-95D6-B2BD6D52CBDD}" name="Tabla1" displayName="Tabla1" ref="D3:F23" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="D3:F23" xr:uid="{FDFFDC23-1EA5-434F-95D6-B2BD6D52CBDD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FDFFDC23-1EA5-434F-95D6-B2BD6D52CBDD}" name="Tabla1" displayName="Tabla1" ref="D3:F21" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="D3:F21" xr:uid="{FDFFDC23-1EA5-434F-95D6-B2BD6D52CBDD}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{844160B8-1ABC-4FDE-A15F-3AFEF16D1615}" name="Fecha" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{A5E8FD62-FCE4-4FAF-B364-C9A1B846CE91}" name="Tarea" dataDxfId="1"/>
@@ -1267,10 +1287,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:J47"/>
+  <dimension ref="B1:J45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1519,9 +1539,15 @@
     </row>
     <row r="17" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="24"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
+      <c r="D17" s="19">
+        <v>45430</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="20">
+        <v>5</v>
+      </c>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
@@ -1542,7 +1568,9 @@
       <c r="I18" s="4"/>
     </row>
     <row r="19" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="26"/>
+      <c r="B19" s="30" t="s">
+        <v>18</v>
+      </c>
       <c r="D19" s="25">
         <v>45412</v>
       </c>
@@ -1558,51 +1586,59 @@
     </row>
     <row r="20" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="27"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
+      <c r="D20" s="25">
+        <v>45430</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="26">
+        <v>3</v>
+      </c>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
     </row>
     <row r="21" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="25"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
+      <c r="B21" s="27"/>
+      <c r="D21" s="25">
+        <v>45431</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="26">
+        <v>2</v>
+      </c>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
     </row>
     <row r="22" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="26"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
+      <c r="D22" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="21"/>
+      <c r="F22" s="23">
+        <f>SUBTOTAL(109,Tabla1[Horas])</f>
+        <v>50.5</v>
+      </c>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
     </row>
     <row r="23" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="26"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
     </row>
     <row r="24" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D24" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="21"/>
-      <c r="F24" s="23">
-        <f>SUBTOTAL(109,Tabla1[Horas])</f>
-        <v>40.5</v>
-      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
@@ -1723,16 +1759,6 @@
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
-    </row>
-    <row r="46" spans="4:6" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-    </row>
-    <row r="47" spans="4:6" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1757,24 +1783,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DEEA25CC0A0AC24199CDC46C25B8B0BC" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e3b47856d4cf355c0dacb39e1084d14f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="6dc4bcd6-49db-4c07-9060-8acfc67cef9f" xmlns:ns3="fb0879af-3eba-417a-a55a-ffe6dcd6ca77" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a845a615265fdb1f7b12cc65ac20ecbd" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1982,10 +1990,40 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE17AD16-C3BD-472A-B362-8A85F95573CA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1227E31-123E-44EE-A422-2705DF3A5917}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="6dc4bcd6-49db-4c07-9060-8acfc67cef9f"/>
+    <ds:schemaRef ds:uri="fb0879af-3eba-417a-a55a-ffe6dcd6ca77"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2009,21 +2047,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1227E31-123E-44EE-A422-2705DF3A5917}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE17AD16-C3BD-472A-B362-8A85F95573CA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="6dc4bcd6-49db-4c07-9060-8acfc67cef9f"/>
-    <ds:schemaRef ds:uri="fb0879af-3eba-417a-a55a-ffe6dcd6ca77"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>